<commit_message>
add manuais de instalação e fabricação) ;
</commit_message>
<xml_diff>
--- a/projeto-aquisicao-local/banco de dados/banco/documentação/TABELAS BANCO.xlsx
+++ b/projeto-aquisicao-local/banco de dados/banco/documentação/TABELAS BANCO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BANDTEC\8-projeto_2.0\Projeto2.0\projeto-aquisicao-local\banco de dados\banco novo\documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BANDTEC\8-projeto_2.0\Projeto2.0\projeto-aquisicao-local\banco de dados\banco\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD2C339-F1C0-43D4-BC25-4412B0A6DB61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4442464B-0ED5-4320-A1C2-C40D58B8E65E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7920" yWindow="-15030" windowWidth="28800" windowHeight="11835" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="4620" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -976,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AJ57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>

</xml_diff>